<commit_message>
fixes inventory constraint bug
</commit_message>
<xml_diff>
--- a/Phase1-answer/Question2-Part A/Q2Data.xlsx
+++ b/Phase1-answer/Question2-Part A/Q2Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semester 7\Operation Research 2\Project\Answer\Phase1-answer\Question2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Semester 7\Operation Research 2\Project\Answer\Phase1-answer\Question2-Part A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF49D04E-3F08-4309-9DDF-8543397219BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0748E579-F76A-44BB-A7E9-3D1C7237A757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -166,7 +166,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -267,11 +267,11 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -860,7 +860,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -885,20 +885,20 @@
         <v>0</v>
       </c>
       <c r="I4" s="6">
-        <v>199.99999999999994</v>
+        <v>0</v>
       </c>
       <c r="J4" s="6">
-        <v>532.63888888888891</v>
+        <v>659.25925925925924</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>24</v>
       </c>
       <c r="M4" s="5">
-        <v>246493.14236111112</v>
+        <v>240907.40740740742</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -924,17 +924,17 @@
         <v>0</v>
       </c>
       <c r="J5" s="6">
-        <v>467.36111111111114</v>
+        <v>540.74074074074076</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="M5" s="5">
-        <v>54119.531250000007</v>
+        <v>56249.999999999993</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
@@ -948,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="6">
-        <v>32.5</v>
+        <v>0</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -966,11 +966,11 @@
         <v>26</v>
       </c>
       <c r="M6" s="5">
-        <v>104387.32638888888</v>
+        <v>107842.59259259258</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
@@ -984,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="6">
-        <v>37.500000000000341</v>
+        <v>750</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -996,11 +996,11 @@
         <v>0</v>
       </c>
       <c r="J7" s="6">
-        <v>732.03125</v>
+        <v>750</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="6">
-        <v>697.96874999999977</v>
+        <v>0</v>
       </c>
       <c r="H8" s="6">
         <v>0</v>
@@ -1059,7 +1059,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1072,26 +1072,26 @@
         <v>1</v>
       </c>
       <c r="E12" s="6">
+        <v>22.222222222222399</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
         <v>159.25925925925921</v>
       </c>
-      <c r="F12" s="6">
-        <v>127.77777777777777</v>
-      </c>
-      <c r="G12" s="6">
-        <v>106.48148148148151</v>
-      </c>
       <c r="H12" s="6">
-        <v>53.240740740740755</v>
+        <v>159.25925925925921</v>
       </c>
       <c r="I12" s="6">
-        <v>126.62037037037035</v>
+        <v>159.25925925925921</v>
       </c>
       <c r="J12" s="6">
         <v>159.25925925925921</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1102,26 +1102,26 @@
         <v>2</v>
       </c>
       <c r="E13" s="6">
+        <v>177.7777777777776</v>
+      </c>
+      <c r="F13" s="6">
+        <v>200</v>
+      </c>
+      <c r="G13" s="6">
         <v>40.74074074074079</v>
       </c>
-      <c r="F13" s="6">
-        <v>72.222222222222229</v>
-      </c>
-      <c r="G13" s="6">
-        <v>93.518518518518491</v>
-      </c>
       <c r="H13" s="6">
-        <v>146.75925925925924</v>
+        <v>40.74074074074079</v>
       </c>
       <c r="I13" s="6">
-        <v>73.379629629629648</v>
+        <v>40.74074074074079</v>
       </c>
       <c r="J13" s="6">
         <v>40.74074074074079</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1144,14 +1144,14 @@
         <v>0</v>
       </c>
       <c r="I14" s="6">
-        <v>32.5</v>
+        <v>0</v>
       </c>
       <c r="J14" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
@@ -1165,23 +1165,23 @@
         <v>250</v>
       </c>
       <c r="F15" s="6">
-        <v>143.75000000000017</v>
+        <v>250</v>
       </c>
       <c r="G15" s="6">
-        <v>71.875000000000085</v>
+        <v>250</v>
       </c>
       <c r="H15" s="6">
-        <v>35.937500000000043</v>
+        <v>250</v>
       </c>
       <c r="I15" s="6">
-        <v>17.968750000000021</v>
+        <v>250</v>
       </c>
       <c r="J15" s="6">
         <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1195,16 +1195,16 @@
         <v>0</v>
       </c>
       <c r="F16" s="6">
-        <v>106.24999999999984</v>
+        <v>0</v>
       </c>
       <c r="G16" s="6">
-        <v>178.12499999999991</v>
+        <v>0</v>
       </c>
       <c r="H16" s="6">
-        <v>214.06249999999994</v>
+        <v>0</v>
       </c>
       <c r="I16" s="6">
-        <v>199.53124999999997</v>
+        <v>0</v>
       </c>
       <c r="J16" s="6">
         <v>0</v>
@@ -1240,7 +1240,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1253,26 +1253,26 @@
         <v>1</v>
       </c>
       <c r="E20" s="6">
-        <v>340.74074074074076</v>
+        <v>477.7777777777776</v>
       </c>
       <c r="F20" s="6">
-        <v>212.96296296296302</v>
+        <v>477.7777777777776</v>
       </c>
       <c r="G20" s="6">
-        <v>106.48148148148151</v>
+        <v>318.51851851851842</v>
       </c>
       <c r="H20" s="6">
-        <v>53.240740740740755</v>
+        <v>159.25925925925921</v>
       </c>
       <c r="I20" s="6">
-        <v>126.62037037037035</v>
+        <v>0</v>
       </c>
       <c r="J20" s="6">
         <v>500</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1283,26 +1283,26 @@
         <v>2</v>
       </c>
       <c r="E21" s="6">
-        <v>459.25925925925924</v>
+        <v>322.2222222222224</v>
       </c>
       <c r="F21" s="6">
-        <v>387.03703703703701</v>
+        <v>122.2222222222224</v>
       </c>
       <c r="G21" s="6">
-        <v>293.51851851851853</v>
+        <v>81.481481481481609</v>
       </c>
       <c r="H21" s="6">
-        <v>146.7592592592593</v>
+        <v>40.740740740740819</v>
       </c>
       <c r="I21" s="6">
-        <v>73.379629629629648</v>
+        <v>0</v>
       </c>
       <c r="J21" s="6">
         <v>500</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1316,13 +1316,13 @@
         <v>500</v>
       </c>
       <c r="F22" s="6">
-        <v>532.5</v>
+        <v>500</v>
       </c>
       <c r="G22" s="6">
-        <v>532.5</v>
+        <v>500</v>
       </c>
       <c r="H22" s="6">
-        <v>532.5</v>
+        <v>500</v>
       </c>
       <c r="I22" s="6">
         <v>500</v>
@@ -1332,7 +1332,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
@@ -1346,23 +1346,23 @@
         <v>250</v>
       </c>
       <c r="F23" s="6">
-        <v>143.75000000000017</v>
+        <v>750</v>
       </c>
       <c r="G23" s="6">
-        <v>71.875000000000085</v>
+        <v>500</v>
       </c>
       <c r="H23" s="6">
-        <v>35.937500000000043</v>
+        <v>250</v>
       </c>
       <c r="I23" s="6">
-        <v>17.968750000000021</v>
+        <v>0</v>
       </c>
       <c r="J23" s="6">
         <v>500</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
@@ -1376,13 +1376,13 @@
         <v>500</v>
       </c>
       <c r="F24" s="6">
-        <v>393.75000000000017</v>
+        <v>500</v>
       </c>
       <c r="G24" s="6">
-        <v>913.59375</v>
+        <v>500</v>
       </c>
       <c r="H24" s="6">
-        <v>699.53125</v>
+        <v>500</v>
       </c>
       <c r="I24" s="6">
         <v>500</v>
@@ -1445,7 +1445,7 @@
         <f>SUM(J12:J16)* input!$C$9</f>
         <v>67500</v>
       </c>
-      <c r="K28" s="8">
+      <c r="K28" s="7">
         <f>SUM(E28:J28)</f>
         <v>405000</v>
       </c>
@@ -1460,25 +1460,25 @@
       </c>
       <c r="F29" s="6">
         <f t="shared" ref="F29:J29" si="0">SUM(F20:F24)</f>
-        <v>1670.0000000000005</v>
+        <v>2350</v>
       </c>
       <c r="G29" s="6">
         <f t="shared" si="0"/>
-        <v>1917.96875</v>
+        <v>1900</v>
       </c>
       <c r="H29" s="6">
         <f t="shared" si="0"/>
-        <v>1467.96875</v>
+        <v>1450</v>
       </c>
       <c r="I29" s="6">
         <f t="shared" si="0"/>
-        <v>1217.96875</v>
+        <v>1000</v>
       </c>
       <c r="J29" s="6">
         <f t="shared" si="0"/>
         <v>2500</v>
       </c>
-      <c r="K29" s="8" t="s">
+      <c r="K29" s="7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1492,27 +1492,27 @@
       </c>
       <c r="F30" s="1">
         <f>F29*input!$C$12</f>
-        <v>8350.0000000000018</v>
+        <v>11750</v>
       </c>
       <c r="G30" s="1">
         <f>G29*input!$C$12</f>
-        <v>9589.84375</v>
+        <v>9500</v>
       </c>
       <c r="H30" s="1">
         <f>H29*input!$C$12</f>
-        <v>7339.84375</v>
+        <v>7250</v>
       </c>
       <c r="I30" s="1">
         <f>I29*input!$C$12</f>
-        <v>6089.84375</v>
+        <v>5000</v>
       </c>
       <c r="J30" s="1">
         <f>J29*input!$C$12</f>
         <v>12500</v>
       </c>
-      <c r="K30" s="8">
+      <c r="K30" s="7">
         <f t="shared" ref="K30:K32" si="1">SUM(E30:J30)</f>
-        <v>54119.53125</v>
+        <v>56250</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1525,11 +1525,11 @@
       </c>
       <c r="F31" s="1">
         <f>SUMPRODUCT(F4:F8, input!E3:E7)</f>
-        <v>6950.0000000000309</v>
+        <v>67500</v>
       </c>
       <c r="G31" s="1">
         <f>SUMPRODUCT(G4:G8, input!F3:F7)</f>
-        <v>66307.031249999985</v>
+        <v>0</v>
       </c>
       <c r="H31" s="1">
         <f>SUMPRODUCT(H4:H8, input!G3:G7)</f>
@@ -1537,15 +1537,15 @@
       </c>
       <c r="I31" s="1">
         <f>SUMPRODUCT(I4:I8, input!H3:H7)</f>
-        <v>19999.999999999993</v>
+        <v>0</v>
       </c>
       <c r="J31" s="1">
         <f>SUMPRODUCT(J4:J8, input!I3:I7)</f>
-        <v>153236.11111111112</v>
-      </c>
-      <c r="K31" s="8">
+        <v>173407.40740740742</v>
+      </c>
+      <c r="K31" s="7">
         <f t="shared" si="1"/>
-        <v>246493.14236111112</v>
+        <v>240907.40740740742</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1558,27 +1558,27 @@
       </c>
       <c r="F32" s="1">
         <f t="shared" ref="F32:J32" si="2">F28-F30-F31</f>
-        <v>52199.999999999971</v>
+        <v>-11750</v>
       </c>
       <c r="G32" s="1">
         <f t="shared" si="2"/>
-        <v>-8396.8749999999854</v>
+        <v>58000</v>
       </c>
       <c r="H32" s="1">
         <f t="shared" si="2"/>
-        <v>60160.15625</v>
+        <v>60250</v>
       </c>
       <c r="I32" s="1">
         <f t="shared" si="2"/>
-        <v>41410.156250000007</v>
+        <v>62500</v>
       </c>
       <c r="J32" s="1">
         <f t="shared" si="2"/>
-        <v>-98236.111111111124</v>
-      </c>
-      <c r="K32" s="8">
+        <v>-118407.40740740742</v>
+      </c>
+      <c r="K32" s="7">
         <f t="shared" si="1"/>
-        <v>104387.32638888888</v>
+        <v>107842.59259259258</v>
       </c>
     </row>
     <row r="33" spans="4:10" x14ac:dyDescent="0.3">
@@ -1587,11 +1587,11 @@
       </c>
       <c r="E33" s="1">
         <f>SUMPRODUCT(E12:E16, input!$J$3:$J$7)/ SUM(output!E12:E16)</f>
-        <v>6</v>
+        <v>5.1777777777777789</v>
       </c>
       <c r="F33" s="1">
         <f>SUMPRODUCT(F12:F16, input!$J$3:$J$7)/ SUM(output!F12:F16)</f>
-        <v>6</v>
+        <v>5.0444444444444443</v>
       </c>
       <c r="G33" s="1">
         <f>SUMPRODUCT(G12:G16, input!$J$3:$J$7)/ SUM(output!G12:G16)</f>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="H33" s="1">
         <f>SUMPRODUCT(H12:H16, input!$J$3:$J$7)/ SUM(output!H12:H16)</f>
-        <v>5.7444444444444445</v>
+        <v>6</v>
       </c>
       <c r="I33" s="1">
         <f>SUMPRODUCT(I12:I16, input!$J$3:$J$7)/ SUM(output!I12:I16)</f>

</xml_diff>